<commit_message>
chore: actualizar datos y reporte web
</commit_message>
<xml_diff>
--- a/data-coyuntura.xlsx
+++ b/data-coyuntura.xlsx
@@ -31,7 +31,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -40,17 +40,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCED4DA"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,9 +76,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,26 +371,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true">
+      <pane ySplit="1" xSplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>39083</v>
       </c>
       <c r="B2" t="n">
@@ -386,7 +403,7 @@
       <c r="D2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>39114</v>
       </c>
       <c r="B3" t="n">
@@ -396,7 +413,7 @@
       <c r="D3"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>39142</v>
       </c>
       <c r="B4" t="n">
@@ -406,7 +423,7 @@
       <c r="D4"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>39173</v>
       </c>
       <c r="B5" t="n">
@@ -416,7 +433,7 @@
       <c r="D5"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>39203</v>
       </c>
       <c r="B6" t="n">
@@ -426,7 +443,7 @@
       <c r="D6"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>39234</v>
       </c>
       <c r="B7" t="n">
@@ -436,7 +453,7 @@
       <c r="D7"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>39264</v>
       </c>
       <c r="B8" t="n">
@@ -446,7 +463,7 @@
       <c r="D8"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>39295</v>
       </c>
       <c r="B9" t="n">
@@ -456,7 +473,7 @@
       <c r="D9"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>39326</v>
       </c>
       <c r="B10" t="n">
@@ -466,7 +483,7 @@
       <c r="D10"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>39356</v>
       </c>
       <c r="B11" t="n">
@@ -476,7 +493,7 @@
       <c r="D11"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>39387</v>
       </c>
       <c r="B12" t="n">
@@ -486,7 +503,7 @@
       <c r="D12"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>39417</v>
       </c>
       <c r="B13" t="n">
@@ -496,7 +513,7 @@
       <c r="D13"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>39448</v>
       </c>
       <c r="B14" t="n">
@@ -506,7 +523,7 @@
       <c r="D14"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>39479</v>
       </c>
       <c r="B15" t="n">
@@ -516,7 +533,7 @@
       <c r="D15"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>39508</v>
       </c>
       <c r="B16" t="n">
@@ -526,7 +543,7 @@
       <c r="D16"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="2" t="n">
         <v>39539</v>
       </c>
       <c r="B17" t="n">
@@ -536,7 +553,7 @@
       <c r="D17"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <v>39569</v>
       </c>
       <c r="B18" t="n">
@@ -546,7 +563,7 @@
       <c r="D18"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <v>39600</v>
       </c>
       <c r="B19" t="n">
@@ -556,7 +573,7 @@
       <c r="D19"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <v>39630</v>
       </c>
       <c r="B20" t="n">
@@ -566,7 +583,7 @@
       <c r="D20"/>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="2" t="n">
         <v>39661</v>
       </c>
       <c r="B21" t="n">
@@ -576,7 +593,7 @@
       <c r="D21"/>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="2" t="n">
         <v>39692</v>
       </c>
       <c r="B22" t="n">
@@ -586,7 +603,7 @@
       <c r="D22"/>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="2" t="n">
         <v>39722</v>
       </c>
       <c r="B23" t="n">
@@ -596,7 +613,7 @@
       <c r="D23"/>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <v>39753</v>
       </c>
       <c r="B24" t="n">
@@ -606,7 +623,7 @@
       <c r="D24"/>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <v>39783</v>
       </c>
       <c r="B25" t="n">
@@ -616,7 +633,7 @@
       <c r="D25"/>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <v>39814</v>
       </c>
       <c r="B26" t="n">
@@ -626,7 +643,7 @@
       <c r="D26"/>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="2" t="n">
         <v>39845</v>
       </c>
       <c r="B27" t="n">
@@ -636,7 +653,7 @@
       <c r="D27"/>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="2" t="n">
         <v>39873</v>
       </c>
       <c r="B28" t="n">
@@ -646,7 +663,7 @@
       <c r="D28"/>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <v>39904</v>
       </c>
       <c r="B29" t="n">
@@ -656,7 +673,7 @@
       <c r="D29"/>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="2" t="n">
         <v>39934</v>
       </c>
       <c r="B30" t="n">
@@ -666,7 +683,7 @@
       <c r="D30"/>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="2" t="n">
         <v>39965</v>
       </c>
       <c r="B31" t="n">
@@ -676,7 +693,7 @@
       <c r="D31"/>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="2" t="n">
         <v>39995</v>
       </c>
       <c r="B32" t="n">
@@ -686,7 +703,7 @@
       <c r="D32"/>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="n">
         <v>40026</v>
       </c>
       <c r="B33" t="n">
@@ -696,7 +713,7 @@
       <c r="D33"/>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="2" t="n">
         <v>40057</v>
       </c>
       <c r="B34" t="n">
@@ -706,7 +723,7 @@
       <c r="D34"/>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <v>40087</v>
       </c>
       <c r="B35" t="n">
@@ -716,7 +733,7 @@
       <c r="D35"/>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="2" t="n">
         <v>40118</v>
       </c>
       <c r="B36" t="n">
@@ -726,7 +743,7 @@
       <c r="D36"/>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="2" t="n">
         <v>40148</v>
       </c>
       <c r="B37" t="n">
@@ -736,7 +753,7 @@
       <c r="D37"/>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="2" t="n">
         <v>40179</v>
       </c>
       <c r="B38" t="n">
@@ -746,7 +763,7 @@
       <c r="D38"/>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="2" t="n">
         <v>40210</v>
       </c>
       <c r="B39" t="n">
@@ -756,7 +773,7 @@
       <c r="D39"/>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <v>40238</v>
       </c>
       <c r="B40" t="n">
@@ -766,7 +783,7 @@
       <c r="D40"/>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <v>40269</v>
       </c>
       <c r="B41" t="n">
@@ -776,7 +793,7 @@
       <c r="D41"/>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="2" t="n">
         <v>40299</v>
       </c>
       <c r="B42" t="n">
@@ -786,7 +803,7 @@
       <c r="D42"/>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="2" t="n">
         <v>40330</v>
       </c>
       <c r="B43" t="n">
@@ -796,7 +813,7 @@
       <c r="D43"/>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="2" t="n">
         <v>40360</v>
       </c>
       <c r="B44" t="n">
@@ -806,7 +823,7 @@
       <c r="D44"/>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="2" t="n">
         <v>40391</v>
       </c>
       <c r="B45" t="n">
@@ -816,7 +833,7 @@
       <c r="D45"/>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="2" t="n">
         <v>40422</v>
       </c>
       <c r="B46" t="n">
@@ -826,7 +843,7 @@
       <c r="D46"/>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="2" t="n">
         <v>40452</v>
       </c>
       <c r="B47" t="n">
@@ -836,7 +853,7 @@
       <c r="D47"/>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="2" t="n">
         <v>40483</v>
       </c>
       <c r="B48" t="n">
@@ -846,7 +863,7 @@
       <c r="D48"/>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="2" t="n">
         <v>40513</v>
       </c>
       <c r="B49" t="n">
@@ -856,7 +873,7 @@
       <c r="D49"/>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="2" t="n">
         <v>40544</v>
       </c>
       <c r="B50" t="n">
@@ -866,7 +883,7 @@
       <c r="D50"/>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="2" t="n">
         <v>40575</v>
       </c>
       <c r="B51" t="n">
@@ -876,7 +893,7 @@
       <c r="D51"/>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="2" t="n">
         <v>40603</v>
       </c>
       <c r="B52" t="n">
@@ -886,7 +903,7 @@
       <c r="D52"/>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="2" t="n">
         <v>40634</v>
       </c>
       <c r="B53" t="n">
@@ -896,7 +913,7 @@
       <c r="D53"/>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="2" t="n">
         <v>40664</v>
       </c>
       <c r="B54" t="n">
@@ -906,7 +923,7 @@
       <c r="D54"/>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="2" t="n">
         <v>40695</v>
       </c>
       <c r="B55" t="n">
@@ -916,7 +933,7 @@
       <c r="D55"/>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="2" t="n">
         <v>40725</v>
       </c>
       <c r="B56" t="n">
@@ -926,7 +943,7 @@
       <c r="D56"/>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="2" t="n">
         <v>40756</v>
       </c>
       <c r="B57" t="n">
@@ -936,7 +953,7 @@
       <c r="D57"/>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="2" t="n">
         <v>40787</v>
       </c>
       <c r="B58" t="n">
@@ -946,7 +963,7 @@
       <c r="D58"/>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="2" t="n">
         <v>40817</v>
       </c>
       <c r="B59" t="n">
@@ -956,7 +973,7 @@
       <c r="D59"/>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="2" t="n">
         <v>40848</v>
       </c>
       <c r="B60" t="n">
@@ -966,7 +983,7 @@
       <c r="D60"/>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="2" t="n">
         <v>40878</v>
       </c>
       <c r="B61" t="n">
@@ -976,7 +993,7 @@
       <c r="D61"/>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="2" t="n">
         <v>40909</v>
       </c>
       <c r="B62" t="n">
@@ -986,7 +1003,7 @@
       <c r="D62"/>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="2" t="n">
         <v>40940</v>
       </c>
       <c r="B63" t="n">
@@ -996,7 +1013,7 @@
       <c r="D63"/>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="2" t="n">
         <v>40969</v>
       </c>
       <c r="B64" t="n">
@@ -1006,7 +1023,7 @@
       <c r="D64"/>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="2" t="n">
         <v>41000</v>
       </c>
       <c r="B65" t="n">
@@ -1016,7 +1033,7 @@
       <c r="D65"/>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="2" t="n">
         <v>41030</v>
       </c>
       <c r="B66" t="n">
@@ -1026,7 +1043,7 @@
       <c r="D66"/>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="2" t="n">
         <v>41061</v>
       </c>
       <c r="B67" t="n">
@@ -1036,7 +1053,7 @@
       <c r="D67"/>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="2" t="n">
         <v>41091</v>
       </c>
       <c r="B68" t="n">
@@ -1046,7 +1063,7 @@
       <c r="D68"/>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="2" t="n">
         <v>41122</v>
       </c>
       <c r="B69" t="n">
@@ -1056,7 +1073,7 @@
       <c r="D69"/>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="2" t="n">
         <v>41153</v>
       </c>
       <c r="B70" t="n">
@@ -1066,7 +1083,7 @@
       <c r="D70"/>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="2" t="n">
         <v>41183</v>
       </c>
       <c r="B71" t="n">
@@ -1076,7 +1093,7 @@
       <c r="D71"/>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="2" t="n">
         <v>41214</v>
       </c>
       <c r="B72" t="n">
@@ -1086,7 +1103,7 @@
       <c r="D72"/>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="2" t="n">
         <v>41244</v>
       </c>
       <c r="B73" t="n">
@@ -1096,7 +1113,7 @@
       <c r="D73"/>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="2" t="n">
         <v>41275</v>
       </c>
       <c r="B74" t="n">
@@ -1106,7 +1123,7 @@
       <c r="D74"/>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="2" t="n">
         <v>41306</v>
       </c>
       <c r="B75" t="n">
@@ -1116,7 +1133,7 @@
       <c r="D75"/>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="2" t="n">
         <v>41334</v>
       </c>
       <c r="B76" t="n">
@@ -1126,7 +1143,7 @@
       <c r="D76"/>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="2" t="n">
         <v>41365</v>
       </c>
       <c r="B77" t="n">
@@ -1136,7 +1153,7 @@
       <c r="D77"/>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="2" t="n">
         <v>41395</v>
       </c>
       <c r="B78" t="n">
@@ -1146,7 +1163,7 @@
       <c r="D78"/>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="2" t="n">
         <v>41426</v>
       </c>
       <c r="B79" t="n">
@@ -1156,7 +1173,7 @@
       <c r="D79"/>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="2" t="n">
         <v>41456</v>
       </c>
       <c r="B80" t="n">
@@ -1166,7 +1183,7 @@
       <c r="D80"/>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="2" t="n">
         <v>41487</v>
       </c>
       <c r="B81" t="n">
@@ -1176,7 +1193,7 @@
       <c r="D81"/>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="2" t="n">
         <v>41518</v>
       </c>
       <c r="B82" t="n">
@@ -1186,7 +1203,7 @@
       <c r="D82"/>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="2" t="n">
         <v>41548</v>
       </c>
       <c r="B83" t="n">
@@ -1196,7 +1213,7 @@
       <c r="D83"/>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="2" t="n">
         <v>41579</v>
       </c>
       <c r="B84" t="n">
@@ -1206,7 +1223,7 @@
       <c r="D84"/>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="2" t="n">
         <v>41609</v>
       </c>
       <c r="B85" t="n">
@@ -1216,7 +1233,7 @@
       <c r="D85"/>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="2" t="n">
         <v>41640</v>
       </c>
       <c r="B86" t="n">
@@ -1226,7 +1243,7 @@
       <c r="D86"/>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="2" t="n">
         <v>41671</v>
       </c>
       <c r="B87" t="n">
@@ -1236,7 +1253,7 @@
       <c r="D87"/>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="2" t="n">
         <v>41699</v>
       </c>
       <c r="B88" t="n">
@@ -1246,7 +1263,7 @@
       <c r="D88"/>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="2" t="n">
         <v>41730</v>
       </c>
       <c r="B89" t="n">
@@ -1256,7 +1273,7 @@
       <c r="D89"/>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="2" t="n">
         <v>41760</v>
       </c>
       <c r="B90" t="n">
@@ -1266,7 +1283,7 @@
       <c r="D90"/>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="2" t="n">
         <v>41791</v>
       </c>
       <c r="B91" t="n">
@@ -1276,7 +1293,7 @@
       <c r="D91"/>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="2" t="n">
         <v>41821</v>
       </c>
       <c r="B92" t="n">
@@ -1286,7 +1303,7 @@
       <c r="D92"/>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="2" t="n">
         <v>41852</v>
       </c>
       <c r="B93" t="n">
@@ -1296,7 +1313,7 @@
       <c r="D93"/>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="2" t="n">
         <v>41883</v>
       </c>
       <c r="B94" t="n">
@@ -1306,7 +1323,7 @@
       <c r="D94"/>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="B95" t="n">
@@ -1316,7 +1333,7 @@
       <c r="D95"/>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="2" t="n">
         <v>41944</v>
       </c>
       <c r="B96" t="n">
@@ -1326,7 +1343,7 @@
       <c r="D96"/>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="2" t="n">
         <v>41974</v>
       </c>
       <c r="B97" t="n">
@@ -1340,7 +1357,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="2" t="n">
         <v>42005</v>
       </c>
       <c r="B98" t="n">
@@ -1354,7 +1371,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="2" t="n">
         <v>42036</v>
       </c>
       <c r="B99" t="n">
@@ -1368,7 +1385,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="2" t="n">
         <v>42064</v>
       </c>
       <c r="B100" t="n">
@@ -1382,7 +1399,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="2" t="n">
         <v>42095</v>
       </c>
       <c r="B101" t="n">
@@ -1396,7 +1413,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="2" t="n">
         <v>42125</v>
       </c>
       <c r="B102" t="n">
@@ -1410,7 +1427,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="2" t="n">
         <v>42156</v>
       </c>
       <c r="B103" t="n">
@@ -1424,7 +1441,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="2" t="n">
         <v>42186</v>
       </c>
       <c r="B104" t="n">
@@ -1438,7 +1455,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="2" t="n">
         <v>42217</v>
       </c>
       <c r="B105" t="n">
@@ -1452,7 +1469,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="2" t="n">
         <v>42248</v>
       </c>
       <c r="B106" t="n">
@@ -1466,7 +1483,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="2" t="n">
         <v>42278</v>
       </c>
       <c r="B107" t="n">
@@ -1480,7 +1497,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="2" t="n">
         <v>42309</v>
       </c>
       <c r="B108" t="n">
@@ -1494,7 +1511,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="2" t="n">
         <v>42339</v>
       </c>
       <c r="B109" t="n">
@@ -1508,7 +1525,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="2" t="n">
         <v>42370</v>
       </c>
       <c r="B110" t="n">
@@ -1522,7 +1539,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="2" t="n">
         <v>42401</v>
       </c>
       <c r="B111" t="n">
@@ -1536,7 +1553,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="2" t="n">
         <v>42430</v>
       </c>
       <c r="B112" t="n">
@@ -1550,7 +1567,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="2" t="n">
         <v>42461</v>
       </c>
       <c r="B113" t="n">
@@ -1564,7 +1581,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="2" t="n">
         <v>42491</v>
       </c>
       <c r="B114" t="n">
@@ -1578,7 +1595,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="2" t="n">
         <v>42522</v>
       </c>
       <c r="B115" t="n">
@@ -1592,7 +1609,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="2" t="n">
         <v>42552</v>
       </c>
       <c r="B116" t="n">
@@ -1606,7 +1623,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="2" t="n">
         <v>42583</v>
       </c>
       <c r="B117" t="n">
@@ -1620,7 +1637,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="2" t="n">
         <v>42614</v>
       </c>
       <c r="B118" t="n">
@@ -1634,7 +1651,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="2" t="n">
         <v>42644</v>
       </c>
       <c r="B119" t="n">
@@ -1648,7 +1665,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="2" t="n">
         <v>42675</v>
       </c>
       <c r="B120" t="n">
@@ -1662,7 +1679,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="2" t="n">
         <v>42705</v>
       </c>
       <c r="B121" t="n">
@@ -1676,7 +1693,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="2" t="n">
         <v>42736</v>
       </c>
       <c r="B122" t="n">
@@ -1690,7 +1707,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="2" t="n">
         <v>42767</v>
       </c>
       <c r="B123" t="n">
@@ -1704,7 +1721,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="n">
+      <c r="A124" s="2" t="n">
         <v>42795</v>
       </c>
       <c r="B124" t="n">
@@ -1718,7 +1735,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="n">
+      <c r="A125" s="2" t="n">
         <v>42826</v>
       </c>
       <c r="B125" t="n">
@@ -1732,7 +1749,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="n">
+      <c r="A126" s="2" t="n">
         <v>42856</v>
       </c>
       <c r="B126" t="n">
@@ -1746,7 +1763,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="n">
+      <c r="A127" s="2" t="n">
         <v>42887</v>
       </c>
       <c r="B127" t="n">
@@ -1760,7 +1777,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="n">
+      <c r="A128" s="2" t="n">
         <v>42917</v>
       </c>
       <c r="B128" t="n">
@@ -1774,7 +1791,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="n">
+      <c r="A129" s="2" t="n">
         <v>42948</v>
       </c>
       <c r="B129" t="n">
@@ -1788,7 +1805,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="n">
+      <c r="A130" s="2" t="n">
         <v>42979</v>
       </c>
       <c r="B130" t="n">
@@ -1802,7 +1819,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="n">
+      <c r="A131" s="2" t="n">
         <v>43009</v>
       </c>
       <c r="B131" t="n">
@@ -1816,7 +1833,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="n">
+      <c r="A132" s="2" t="n">
         <v>43040</v>
       </c>
       <c r="B132" t="n">
@@ -1830,7 +1847,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="1" t="n">
+      <c r="A133" s="2" t="n">
         <v>43070</v>
       </c>
       <c r="B133" t="n">
@@ -1844,7 +1861,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="n">
+      <c r="A134" s="2" t="n">
         <v>43101</v>
       </c>
       <c r="B134" t="n">
@@ -1858,7 +1875,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="n">
+      <c r="A135" s="2" t="n">
         <v>43132</v>
       </c>
       <c r="B135" t="n">
@@ -1872,7 +1889,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="n">
+      <c r="A136" s="2" t="n">
         <v>43160</v>
       </c>
       <c r="B136" t="n">
@@ -1886,7 +1903,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="1" t="n">
+      <c r="A137" s="2" t="n">
         <v>43191</v>
       </c>
       <c r="B137" t="n">
@@ -1900,7 +1917,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="n">
+      <c r="A138" s="2" t="n">
         <v>43221</v>
       </c>
       <c r="B138" t="n">
@@ -1914,7 +1931,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="n">
+      <c r="A139" s="2" t="n">
         <v>43252</v>
       </c>
       <c r="B139" t="n">
@@ -1928,7 +1945,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="1" t="n">
+      <c r="A140" s="2" t="n">
         <v>43282</v>
       </c>
       <c r="B140" t="n">
@@ -1942,7 +1959,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="n">
+      <c r="A141" s="2" t="n">
         <v>43313</v>
       </c>
       <c r="B141" t="n">
@@ -1956,7 +1973,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="n">
+      <c r="A142" s="2" t="n">
         <v>43344</v>
       </c>
       <c r="B142" t="n">
@@ -1970,7 +1987,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="1" t="n">
+      <c r="A143" s="2" t="n">
         <v>43374</v>
       </c>
       <c r="B143" t="n">
@@ -1984,7 +2001,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="1" t="n">
+      <c r="A144" s="2" t="n">
         <v>43405</v>
       </c>
       <c r="B144" t="n">
@@ -1998,7 +2015,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="n">
+      <c r="A145" s="2" t="n">
         <v>43435</v>
       </c>
       <c r="B145" t="n">
@@ -2012,7 +2029,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="1" t="n">
+      <c r="A146" s="2" t="n">
         <v>43466</v>
       </c>
       <c r="B146" t="n">
@@ -2026,7 +2043,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="1" t="n">
+      <c r="A147" s="2" t="n">
         <v>43497</v>
       </c>
       <c r="B147" t="n">
@@ -2040,7 +2057,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="1" t="n">
+      <c r="A148" s="2" t="n">
         <v>43525</v>
       </c>
       <c r="B148" t="n">
@@ -2054,7 +2071,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="1" t="n">
+      <c r="A149" s="2" t="n">
         <v>43556</v>
       </c>
       <c r="B149" t="n">
@@ -2068,7 +2085,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="1" t="n">
+      <c r="A150" s="2" t="n">
         <v>43586</v>
       </c>
       <c r="B150" t="n">
@@ -2082,7 +2099,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="1" t="n">
+      <c r="A151" s="2" t="n">
         <v>43617</v>
       </c>
       <c r="B151" t="n">
@@ -2096,7 +2113,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="1" t="n">
+      <c r="A152" s="2" t="n">
         <v>43647</v>
       </c>
       <c r="B152" t="n">
@@ -2110,7 +2127,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="1" t="n">
+      <c r="A153" s="2" t="n">
         <v>43678</v>
       </c>
       <c r="B153" t="n">
@@ -2124,7 +2141,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="1" t="n">
+      <c r="A154" s="2" t="n">
         <v>43709</v>
       </c>
       <c r="B154" t="n">
@@ -2138,7 +2155,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="1" t="n">
+      <c r="A155" s="2" t="n">
         <v>43739</v>
       </c>
       <c r="B155" t="n">
@@ -2152,7 +2169,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="1" t="n">
+      <c r="A156" s="2" t="n">
         <v>43770</v>
       </c>
       <c r="B156" t="n">
@@ -2166,7 +2183,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="1" t="n">
+      <c r="A157" s="2" t="n">
         <v>43800</v>
       </c>
       <c r="B157" t="n">
@@ -2180,7 +2197,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="1" t="n">
+      <c r="A158" s="2" t="n">
         <v>43831</v>
       </c>
       <c r="B158" t="n">
@@ -2194,7 +2211,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="1" t="n">
+      <c r="A159" s="2" t="n">
         <v>43862</v>
       </c>
       <c r="B159" t="n">
@@ -2208,7 +2225,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="1" t="n">
+      <c r="A160" s="2" t="n">
         <v>43891</v>
       </c>
       <c r="B160" t="n">
@@ -2222,7 +2239,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="1" t="n">
+      <c r="A161" s="2" t="n">
         <v>43922</v>
       </c>
       <c r="B161" t="n">
@@ -2236,7 +2253,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="1" t="n">
+      <c r="A162" s="2" t="n">
         <v>43952</v>
       </c>
       <c r="B162" t="n">
@@ -2250,7 +2267,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="1" t="n">
+      <c r="A163" s="2" t="n">
         <v>43983</v>
       </c>
       <c r="B163" t="n">
@@ -2264,7 +2281,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="1" t="n">
+      <c r="A164" s="2" t="n">
         <v>44013</v>
       </c>
       <c r="B164" t="n">
@@ -2278,7 +2295,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="1" t="n">
+      <c r="A165" s="2" t="n">
         <v>44044</v>
       </c>
       <c r="B165" t="n">
@@ -2292,7 +2309,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="1" t="n">
+      <c r="A166" s="2" t="n">
         <v>44075</v>
       </c>
       <c r="B166" t="n">
@@ -2306,7 +2323,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="1" t="n">
+      <c r="A167" s="2" t="n">
         <v>44105</v>
       </c>
       <c r="B167" t="n">
@@ -2320,7 +2337,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="1" t="n">
+      <c r="A168" s="2" t="n">
         <v>44136</v>
       </c>
       <c r="B168" t="n">
@@ -2334,7 +2351,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="1" t="n">
+      <c r="A169" s="2" t="n">
         <v>44166</v>
       </c>
       <c r="B169" t="n">
@@ -2348,7 +2365,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="1" t="n">
+      <c r="A170" s="2" t="n">
         <v>44197</v>
       </c>
       <c r="B170" t="n">
@@ -2362,7 +2379,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="1" t="n">
+      <c r="A171" s="2" t="n">
         <v>44228</v>
       </c>
       <c r="B171" t="n">
@@ -2376,7 +2393,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="1" t="n">
+      <c r="A172" s="2" t="n">
         <v>44256</v>
       </c>
       <c r="B172" t="n">
@@ -2390,7 +2407,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="1" t="n">
+      <c r="A173" s="2" t="n">
         <v>44287</v>
       </c>
       <c r="B173" t="n">
@@ -2404,7 +2421,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="1" t="n">
+      <c r="A174" s="2" t="n">
         <v>44317</v>
       </c>
       <c r="B174" t="n">
@@ -2418,7 +2435,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="1" t="n">
+      <c r="A175" s="2" t="n">
         <v>44348</v>
       </c>
       <c r="B175" t="n">
@@ -2432,7 +2449,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="1" t="n">
+      <c r="A176" s="2" t="n">
         <v>44378</v>
       </c>
       <c r="B176" t="n">
@@ -2446,7 +2463,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="1" t="n">
+      <c r="A177" s="2" t="n">
         <v>44409</v>
       </c>
       <c r="B177" t="n">
@@ -2460,7 +2477,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="1" t="n">
+      <c r="A178" s="2" t="n">
         <v>44440</v>
       </c>
       <c r="B178" t="n">
@@ -2474,7 +2491,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="1" t="n">
+      <c r="A179" s="2" t="n">
         <v>44470</v>
       </c>
       <c r="B179" t="n">
@@ -2488,7 +2505,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="1" t="n">
+      <c r="A180" s="2" t="n">
         <v>44501</v>
       </c>
       <c r="B180" t="n">
@@ -2502,7 +2519,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="1" t="n">
+      <c r="A181" s="2" t="n">
         <v>44531</v>
       </c>
       <c r="B181" t="n">
@@ -2516,7 +2533,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="1" t="n">
+      <c r="A182" s="2" t="n">
         <v>44562</v>
       </c>
       <c r="B182" t="n">
@@ -2530,7 +2547,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="1" t="n">
+      <c r="A183" s="2" t="n">
         <v>44593</v>
       </c>
       <c r="B183" t="n">
@@ -2544,7 +2561,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="1" t="n">
+      <c r="A184" s="2" t="n">
         <v>44621</v>
       </c>
       <c r="B184" t="n">
@@ -2558,7 +2575,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="1" t="n">
+      <c r="A185" s="2" t="n">
         <v>44652</v>
       </c>
       <c r="B185" t="n">
@@ -2572,7 +2589,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="1" t="n">
+      <c r="A186" s="2" t="n">
         <v>44682</v>
       </c>
       <c r="B186" t="n">
@@ -2586,7 +2603,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="1" t="n">
+      <c r="A187" s="2" t="n">
         <v>44713</v>
       </c>
       <c r="B187" t="n">
@@ -2600,7 +2617,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="1" t="n">
+      <c r="A188" s="2" t="n">
         <v>44743</v>
       </c>
       <c r="B188" t="n">
@@ -2614,7 +2631,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="1" t="n">
+      <c r="A189" s="2" t="n">
         <v>44774</v>
       </c>
       <c r="B189" t="n">
@@ -2628,7 +2645,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="1" t="n">
+      <c r="A190" s="2" t="n">
         <v>44805</v>
       </c>
       <c r="B190" t="n">
@@ -2642,7 +2659,7 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="1" t="n">
+      <c r="A191" s="2" t="n">
         <v>44835</v>
       </c>
       <c r="B191" t="n">
@@ -2656,7 +2673,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="1" t="n">
+      <c r="A192" s="2" t="n">
         <v>44866</v>
       </c>
       <c r="B192" t="n">
@@ -2670,7 +2687,7 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="1" t="n">
+      <c r="A193" s="2" t="n">
         <v>44896</v>
       </c>
       <c r="B193" t="n">
@@ -2684,7 +2701,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="1" t="n">
+      <c r="A194" s="2" t="n">
         <v>44927</v>
       </c>
       <c r="B194" t="n">
@@ -2698,7 +2715,7 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="1" t="n">
+      <c r="A195" s="2" t="n">
         <v>44958</v>
       </c>
       <c r="B195" t="n">
@@ -2712,7 +2729,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="1" t="n">
+      <c r="A196" s="2" t="n">
         <v>44986</v>
       </c>
       <c r="B196" t="n">
@@ -2726,7 +2743,7 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="1" t="n">
+      <c r="A197" s="2" t="n">
         <v>45017</v>
       </c>
       <c r="B197" t="n">
@@ -2740,7 +2757,7 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="1" t="n">
+      <c r="A198" s="2" t="n">
         <v>45047</v>
       </c>
       <c r="B198" t="n">
@@ -2754,7 +2771,7 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="1" t="n">
+      <c r="A199" s="2" t="n">
         <v>45078</v>
       </c>
       <c r="B199" t="n">
@@ -2768,7 +2785,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="1" t="n">
+      <c r="A200" s="2" t="n">
         <v>45108</v>
       </c>
       <c r="B200" t="n">
@@ -2782,7 +2799,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="1" t="n">
+      <c r="A201" s="2" t="n">
         <v>45139</v>
       </c>
       <c r="B201" t="n">
@@ -2796,7 +2813,7 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="1" t="n">
+      <c r="A202" s="2" t="n">
         <v>45170</v>
       </c>
       <c r="B202" t="n">
@@ -2810,7 +2827,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="1" t="n">
+      <c r="A203" s="2" t="n">
         <v>45200</v>
       </c>
       <c r="B203" t="n">
@@ -2824,7 +2841,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="1" t="n">
+      <c r="A204" s="2" t="n">
         <v>45231</v>
       </c>
       <c r="B204" t="n">
@@ -2838,7 +2855,7 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="1" t="n">
+      <c r="A205" s="2" t="n">
         <v>45261</v>
       </c>
       <c r="B205" t="n">
@@ -2852,7 +2869,7 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="1" t="n">
+      <c r="A206" s="2" t="n">
         <v>45292</v>
       </c>
       <c r="B206" t="n">
@@ -2866,7 +2883,7 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="1" t="n">
+      <c r="A207" s="2" t="n">
         <v>45323</v>
       </c>
       <c r="B207" t="n">
@@ -2880,7 +2897,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="1" t="n">
+      <c r="A208" s="2" t="n">
         <v>45352</v>
       </c>
       <c r="B208" t="n">
@@ -2894,7 +2911,7 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="1" t="n">
+      <c r="A209" s="2" t="n">
         <v>45383</v>
       </c>
       <c r="B209" t="n">
@@ -2908,7 +2925,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="1" t="n">
+      <c r="A210" s="2" t="n">
         <v>45413</v>
       </c>
       <c r="B210" t="n">
@@ -2922,7 +2939,7 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="1" t="n">
+      <c r="A211" s="2" t="n">
         <v>45444</v>
       </c>
       <c r="B211" t="n">
@@ -2936,7 +2953,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="1" t="n">
+      <c r="A212" s="2" t="n">
         <v>45474</v>
       </c>
       <c r="B212" t="n">
@@ -2950,7 +2967,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="1" t="n">
+      <c r="A213" s="2" t="n">
         <v>45505</v>
       </c>
       <c r="B213" t="n">
@@ -2964,7 +2981,7 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="1" t="n">
+      <c r="A214" s="2" t="n">
         <v>45536</v>
       </c>
       <c r="B214" t="n">
@@ -2978,7 +2995,7 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="1" t="n">
+      <c r="A215" s="2" t="n">
         <v>45566</v>
       </c>
       <c r="B215" t="n">
@@ -2992,7 +3009,7 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="1" t="n">
+      <c r="A216" s="2" t="n">
         <v>45597</v>
       </c>
       <c r="B216" t="n">
@@ -3006,7 +3023,7 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="1" t="n">
+      <c r="A217" s="2" t="n">
         <v>45627</v>
       </c>
       <c r="B217" t="n">
@@ -3020,7 +3037,7 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="1" t="n">
+      <c r="A218" s="2" t="n">
         <v>45658</v>
       </c>
       <c r="B218" t="n">
@@ -3034,7 +3051,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="1" t="n">
+      <c r="A219" s="2" t="n">
         <v>45689</v>
       </c>
       <c r="B219" t="n">
@@ -3048,7 +3065,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="1" t="n">
+      <c r="A220" s="2" t="n">
         <v>45717</v>
       </c>
       <c r="B220" t="n">
@@ -3062,7 +3079,7 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="1" t="n">
+      <c r="A221" s="2" t="n">
         <v>45748</v>
       </c>
       <c r="B221" t="n">
@@ -3076,7 +3093,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="1" t="n">
+      <c r="A222" s="2" t="n">
         <v>45778</v>
       </c>
       <c r="B222" t="n">
@@ -3090,7 +3107,7 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="1" t="n">
+      <c r="A223" s="2" t="n">
         <v>45809</v>
       </c>
       <c r="B223" t="n">
@@ -3104,7 +3121,7 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="1" t="n">
+      <c r="A224" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="B224" t="n">
@@ -3118,7 +3135,7 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="1" t="n">
+      <c r="A225" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="B225" t="n">
@@ -3132,7 +3149,7 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="1" t="n">
+      <c r="A226" s="2" t="n">
         <v>45901</v>
       </c>
       <c r="B226" t="n">
@@ -3146,7 +3163,7 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="1" t="n">
+      <c r="A227" s="2" t="n">
         <v>45931</v>
       </c>
       <c r="B227" t="n">

</xml_diff>